<commit_message>
Migrate to JSON-to-SQLite hybrid system
</commit_message>
<xml_diff>
--- a/data-vault/data/web/employer-suite.xlsx
+++ b/data-vault/data/web/employer-suite.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1842,9 +1842,189 @@
         <v>demo job {{TIMESTAMP}} edit</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C73" t="str">
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <v>login_to_employer_portal</v>
+      </c>
+      <c r="E73" t="str">
+        <v/>
+      </c>
+      <c r="F73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C74" t="str">
+        <v>2</v>
+      </c>
+      <c r="D74" t="str">
+        <v>click</v>
+      </c>
+      <c r="E74" t="str">
+        <v>RECENT_INTERNSHIPS_LINK</v>
+      </c>
+      <c r="F74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C75" t="str">
+        <v>3</v>
+      </c>
+      <c r="D75" t="str">
+        <v>waitfor</v>
+      </c>
+      <c r="E75" t="str">
+        <v>EDIT_JOB_BTN</v>
+      </c>
+      <c r="F75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C76" t="str">
+        <v>4</v>
+      </c>
+      <c r="D76" t="str">
+        <v>click</v>
+      </c>
+      <c r="E76" t="str">
+        <v>EDIT_JOB_BTN</v>
+      </c>
+      <c r="F76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C77" t="str">
+        <v>5</v>
+      </c>
+      <c r="D77" t="str">
+        <v>waitfor</v>
+      </c>
+      <c r="E77" t="str">
+        <v>INTERNSHIP_TITLE_INPUT</v>
+      </c>
+      <c r="F77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C78" t="str">
+        <v>6</v>
+      </c>
+      <c r="D78" t="str">
+        <v>type</v>
+      </c>
+      <c r="E78" t="str">
+        <v>INTERNSHIP_TITLE_INPUT</v>
+      </c>
+      <c r="F78" t="str">
+        <v>demo internship {{TIMESTAMP}} edit</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C79" t="str">
+        <v>7</v>
+      </c>
+      <c r="D79" t="str">
+        <v>click</v>
+      </c>
+      <c r="E79" t="str">
+        <v>UPDATE_INTERNSHIP_BTN</v>
+      </c>
+      <c r="F79" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C80" t="str">
+        <v>8</v>
+      </c>
+      <c r="D80" t="str">
+        <v>click</v>
+      </c>
+      <c r="E80" t="str">
+        <v>ALERT_OK_BTN</v>
+      </c>
+      <c r="F80" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>TC009</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Verify Edit Internship Title</v>
+      </c>
+      <c r="C81" t="str">
+        <v>9</v>
+      </c>
+      <c r="D81" t="str">
+        <v>verify_text</v>
+      </c>
+      <c r="E81" t="str">
+        <v>css:body</v>
+      </c>
+      <c r="F81" t="str">
+        <v>demo internship {{TIMESTAMP}} edit</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F72"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F81"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>